<commit_message>
feat: update maintain to viewpoint
</commit_message>
<xml_diff>
--- a/app_PointCloudDataViewer/pointcloud_data_viewer/log/view분석.xlsx
+++ b/app_PointCloudDataViewer/pointcloud_data_viewer/log/view분석.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twchong/workspace/myGithub/flutter_app/app_PointCloudDataViewer/pointcloud_data_viewer/log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77934B7-EA1A-0048-9797-2586670D980F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E524C9-52C6-2A4C-AB73-310C229A816E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18020" yWindow="500" windowWidth="33180" windowHeight="55420" activeTab="2" xr2:uid="{44C6E0C5-C00C-5B41-847D-0E5966727B81}"/>
+    <workbookView xWindow="18020" yWindow="500" windowWidth="33180" windowHeight="34720" activeTab="2" xr2:uid="{44C6E0C5-C00C-5B41-847D-0E5966727B81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15632,10 +15632,15 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:E13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">

</xml_diff>